<commit_message>
Modif affichage des missions
</commit_message>
<xml_diff>
--- a/tableau/6- Annexe 6-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
+++ b/tableau/6- Annexe 6-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\noah-master\tableau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\tp-html\GoncalvesLionel.io\tableau\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9DD06C5-E962-40BB-AA7C-A0BF0D137CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C26FA04-4FAF-4075-9B54-D5BAA266F9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="3720" windowWidth="18900" windowHeight="11770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -659,15 +659,39 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -699,30 +723,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1049,56 +1049,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="24"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:43" ht="41.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="42" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="43"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="30"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
@@ -1110,22 +1110,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="39" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1148,8 +1148,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1205,16 +1205,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1702,16 +1702,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -2064,16 +2064,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="38"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2518,11 +2518,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2530,6 +2525,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>